<commit_message>
Bugfix : Fixing JCG groupstage tracker, replace with a new method. Now same name no longer a problem
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60162E8-FDB6-434D-92D6-D22F54DE21C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B037A304-7B66-444D-A3DF-897FF3FFC6F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="169">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -73,9 +73,6 @@
     <t>72h1S</t>
   </si>
   <si>
-    <t>Evo Lucifer Forest</t>
-  </si>
-  <si>
     <t>Lucifer, Fallen Angel</t>
   </si>
   <si>
@@ -88,12 +85,6 @@
     <t>Sword</t>
   </si>
   <si>
-    <t>Shinobi Tanuki</t>
-  </si>
-  <si>
-    <t>72y7M</t>
-  </si>
-  <si>
     <t>Quickblader</t>
   </si>
   <si>
@@ -172,12 +163,6 @@
     <t>Natura Rune</t>
   </si>
   <si>
-    <t>Magical Augmentation</t>
-  </si>
-  <si>
-    <t>6_X7Q</t>
-  </si>
-  <si>
     <t>Ramp Roost Dragon</t>
   </si>
   <si>
@@ -253,12 +238,6 @@
     <t>748Xg</t>
   </si>
   <si>
-    <t>Abysmal Wraith</t>
-  </si>
-  <si>
-    <t>747oy</t>
-  </si>
-  <si>
     <t>Burial Rite Shadow</t>
   </si>
   <si>
@@ -391,9 +370,6 @@
     <t>6s5My</t>
   </si>
   <si>
-    <t>Control Portal</t>
-  </si>
-  <si>
     <t>Dimension Dominator</t>
   </si>
   <si>
@@ -512,6 +488,45 @@
   </si>
   <si>
     <t>Control Ra Haven</t>
+  </si>
+  <si>
+    <t>Aggro Forest</t>
+  </si>
+  <si>
+    <t>Shamu &amp; Shama, Posh Felines</t>
+  </si>
+  <si>
+    <t>72h1I</t>
+  </si>
+  <si>
+    <t>Stroke of Conviction</t>
+  </si>
+  <si>
+    <t>6xPSQ</t>
+  </si>
+  <si>
+    <t>Control OTK Portal</t>
+  </si>
+  <si>
+    <t>Snnneak Attack!</t>
+  </si>
+  <si>
+    <t>6rc6o</t>
+  </si>
+  <si>
+    <t>Karyl Rune</t>
+  </si>
+  <si>
+    <t>Evo Forest</t>
+  </si>
+  <si>
+    <t>Grudge Teller</t>
+  </si>
+  <si>
+    <t>745MY</t>
+  </si>
+  <si>
+    <t>Midrange Shadow</t>
   </si>
 </sst>
 </file>
@@ -528,11 +543,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -783,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1021"/>
+  <dimension ref="A1:H1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -856,22 +873,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>161</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
@@ -881,23 +898,23 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
+      <c r="C4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
@@ -908,22 +925,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -934,22 +951,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>165</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -960,22 +977,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -986,22 +1003,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -1012,114 +1029,114 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>44</v>
@@ -1128,36 +1145,36 @@
         <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>57</v>
+      <c r="E14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>14</v>
@@ -1168,22 +1185,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>14</v>
@@ -1193,23 +1210,23 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>67</v>
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
@@ -1220,22 +1237,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>14</v>
@@ -1246,22 +1263,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>14</v>
@@ -1271,23 +1288,23 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>78</v>
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>14</v>
@@ -1297,75 +1314,75 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>83</v>
+      <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="G21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>85</v>
+        <v>166</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
@@ -1376,22 +1393,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>140</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>14</v>
@@ -1402,22 +1419,22 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>153</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>14</v>
@@ -1428,100 +1445,100 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>14</v>
+        <v>136</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>90</v>
+        <v>136</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>90</v>
+        <v>134</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>138</v>
+      <c r="A28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
@@ -1532,218 +1549,293 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>14</v>
+        <v>88</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="G34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E36" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="F38" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C38" s="3"/>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C41" s="3"/>
+    </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2721,6 +2813,9 @@
     <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Bugfix : JCG Top16 flexibility and Meta changes
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B037A304-7B66-444D-A3DF-897FF3FFC6F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00225C5C-9057-453F-92EA-23738DB3B12E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="20400" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="164">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -238,24 +238,6 @@
     <t>748Xg</t>
   </si>
   <si>
-    <t>Burial Rite Shadow</t>
-  </si>
-  <si>
-    <t>He Who Once Rocked</t>
-  </si>
-  <si>
-    <t>6yaPS</t>
-  </si>
-  <si>
-    <t>Path to Perdition</t>
-  </si>
-  <si>
-    <t>6uht2</t>
-  </si>
-  <si>
-    <t>Perdition Shadow</t>
-  </si>
-  <si>
     <t>Invincible Monster Trio</t>
   </si>
   <si>
@@ -445,12 +427,6 @@
     <t>Vincent Rune</t>
   </si>
   <si>
-    <t>Magical Gunslinger</t>
-  </si>
-  <si>
-    <t>73PQ2</t>
-  </si>
-  <si>
     <t>Lubelle, Necrofamily</t>
   </si>
   <si>
@@ -460,15 +436,6 @@
     <t>Natura Shadow</t>
   </si>
   <si>
-    <t>Fatal Order</t>
-  </si>
-  <si>
-    <t>gXuCg</t>
-  </si>
-  <si>
-    <t>6yWFg</t>
-  </si>
-  <si>
     <t>Loxis Forest</t>
   </si>
   <si>
@@ -481,12 +448,6 @@
     <t>6-suS</t>
   </si>
   <si>
-    <t>6sp_A</t>
-  </si>
-  <si>
-    <t>Colosseum on High</t>
-  </si>
-  <si>
     <t>Control Ra Haven</t>
   </si>
   <si>
@@ -526,7 +487,31 @@
     <t>745MY</t>
   </si>
   <si>
-    <t>Midrange Shadow</t>
+    <t>Gremory Shadow</t>
+  </si>
+  <si>
+    <t>Gremory, Death Teller</t>
+  </si>
+  <si>
+    <t>6yaPI</t>
+  </si>
+  <si>
+    <t>Valdain Roost Dragon</t>
+  </si>
+  <si>
+    <t>XII. Wolfraud, Hanged Man</t>
+  </si>
+  <si>
+    <t>6-suI</t>
+  </si>
+  <si>
+    <t>Princess Knight</t>
+  </si>
+  <si>
+    <t>6spli</t>
+  </si>
+  <si>
+    <t>Hanged Man Forest</t>
   </si>
 </sst>
 </file>
@@ -800,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1024"/>
+  <dimension ref="A1:H1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -847,22 +832,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>159</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>160</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>161</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>162</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -873,16 +858,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>156</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>157</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>158</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
@@ -899,22 +884,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>154</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
@@ -925,7 +910,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -951,7 +936,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -963,10 +948,10 @@
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -976,23 +961,23 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>22</v>
+      <c r="A7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1009,16 +994,16 @@
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>124</v>
+        <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -1029,22 +1014,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
@@ -1055,126 +1040,126 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>140</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>14</v>
@@ -1185,16 +1170,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>164</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>39</v>
@@ -1210,75 +1195,75 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>14</v>
@@ -1289,22 +1274,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>137</v>
+        <v>55</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>14</v>
@@ -1315,74 +1300,74 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
@@ -1393,22 +1378,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>155</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>14</v>
@@ -1419,22 +1404,22 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>14</v>
@@ -1445,48 +1430,48 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>14</v>
@@ -1497,22 +1482,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>168</v>
+        <v>74</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>14</v>
@@ -1523,100 +1508,100 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>14</v>
+      <c r="G28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="B31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="F31" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>14</v>
@@ -1627,22 +1612,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>14</v>
@@ -1653,23 +1638,23 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1678,23 +1663,23 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>109</v>
+      <c r="A34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
@@ -1705,22 +1690,22 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
@@ -1731,48 +1716,48 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="F37" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
@@ -1783,23 +1768,23 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="G38" s="1" t="s">
         <v>14</v>
       </c>
@@ -1807,35 +1792,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C41" s="3"/>
-    </row>
+    <row r="40" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2815,7 +2775,6 @@
     <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Meta changes and comment removal
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00225C5C-9057-453F-92EA-23738DB3B12E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219EEA30-A16A-4AA8-BFCB-E7D224DAEB52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="20400" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="169">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -512,13 +512,28 @@
   </si>
   <si>
     <t>Hanged Man Forest</t>
+  </si>
+  <si>
+    <t>Mind Splitting AF Portal</t>
+  </si>
+  <si>
+    <t>71VLY</t>
+  </si>
+  <si>
+    <t>Mind Splitter</t>
+  </si>
+  <si>
+    <t>6zcK2</t>
+  </si>
+  <si>
+    <t>Android Artisan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +550,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -563,13 +585,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1789,6 +1813,32 @@
         <v>14</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Feature : Generate JCG Trends
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219EEA30-A16A-4AA8-BFCB-E7D224DAEB52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B8FE76-21A4-4EE3-923A-A97887B19F9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="20400" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="172">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -527,6 +527,15 @@
   </si>
   <si>
     <t>Android Artisan</t>
+  </si>
+  <si>
+    <t>Varmint Hunter</t>
+  </si>
+  <si>
+    <t>72c8y</t>
+  </si>
+  <si>
+    <t>Tempo Storm Forest</t>
   </si>
 </sst>
 </file>
@@ -809,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1023"/>
+  <dimension ref="A1:H1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -985,49 +994,49 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -1053,7 +1062,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
@@ -1064,22 +1073,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -1090,126 +1099,126 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>14</v>
@@ -1220,16 +1229,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>151</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>39</v>
@@ -1245,75 +1254,75 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>52</v>
+      <c r="A17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>158</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>14</v>
@@ -1324,22 +1333,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
@@ -1350,22 +1359,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
@@ -1385,7 +1394,7 @@
         <v>64</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>66</v>
@@ -1401,23 +1410,23 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>73</v>
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>14</v>
@@ -1428,22 +1437,22 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>155</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>71</v>
+        <v>157</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>153</v>
+        <v>72</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>154</v>
+        <v>73</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>14</v>
@@ -1454,42 +1463,42 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>136</v>
+        <v>154</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>129</v>
@@ -1497,31 +1506,31 @@
       <c r="F26" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>14</v>
+      <c r="G26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>14</v>
@@ -1532,48 +1541,48 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" s="2" t="s">
         <v>77</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>76</v>
@@ -1583,49 +1592,49 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>14</v>
@@ -1636,22 +1645,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>150</v>
+        <v>93</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>14</v>
@@ -1662,48 +1671,48 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
@@ -1714,22 +1723,22 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
@@ -1749,7 +1758,7 @@
         <v>106</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>108</v>
@@ -1765,23 +1774,23 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>113</v>
+      <c r="C37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
@@ -1792,22 +1801,22 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>14</v>
@@ -1816,36 +1825,61 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C40" s="3"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C41" s="3"/>
+    </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2825,6 +2859,7 @@
     <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Feature : - Add Unlimited scraper - Change URL hash file to JSON based
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B8FE76-21A4-4EE3-923A-A97887B19F9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6658F-AAF9-422C-90BF-FF24237667C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="300" windowWidth="20400" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="174">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -256,9 +256,6 @@
     <t>74b5o</t>
   </si>
   <si>
-    <t>Corruption Blood</t>
-  </si>
-  <si>
     <t>Baal</t>
   </si>
   <si>
@@ -340,18 +337,6 @@
     <t>Portal</t>
   </si>
   <si>
-    <t>Artifact Scan</t>
-  </si>
-  <si>
-    <t>71TeA</t>
-  </si>
-  <si>
-    <t>Absolute Modesty</t>
-  </si>
-  <si>
-    <t>6s5My</t>
-  </si>
-  <si>
     <t>Dimension Dominator</t>
   </si>
   <si>
@@ -379,9 +364,6 @@
     <t>fskF2</t>
   </si>
   <si>
-    <t>gZ1SK</t>
-  </si>
-  <si>
     <t>6-qS2</t>
   </si>
   <si>
@@ -397,9 +379,6 @@
     <t>74xJg</t>
   </si>
   <si>
-    <t>Illganeau Turbo Portal</t>
-  </si>
-  <si>
     <t>Milteo OTK Shadow</t>
   </si>
   <si>
@@ -514,15 +493,6 @@
     <t>Hanged Man Forest</t>
   </si>
   <si>
-    <t>Mind Splitting AF Portal</t>
-  </si>
-  <si>
-    <t>71VLY</t>
-  </si>
-  <si>
-    <t>Mind Splitter</t>
-  </si>
-  <si>
     <t>6zcK2</t>
   </si>
   <si>
@@ -535,14 +505,50 @@
     <t>72c8y</t>
   </si>
   <si>
-    <t>Tempo Storm Forest</t>
+    <t>Tempo Forest</t>
+  </si>
+  <si>
+    <t>Baal Blood</t>
+  </si>
+  <si>
+    <t>Wrath Blood</t>
+  </si>
+  <si>
+    <t>Scrappy Werewolf</t>
+  </si>
+  <si>
+    <t>74Tn2</t>
+  </si>
+  <si>
+    <t>Darhold, Abyssal Contract</t>
+  </si>
+  <si>
+    <t>70myy</t>
+  </si>
+  <si>
+    <t>Bayleon, Sovereign Light</t>
+  </si>
+  <si>
+    <t>Natura Sword</t>
+  </si>
+  <si>
+    <t>6poty</t>
+  </si>
+  <si>
+    <t>6zhxQ</t>
+  </si>
+  <si>
+    <t>Rebel Against Fate</t>
+  </si>
+  <si>
+    <t>Illganeau Portal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,29 +563,16 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -594,15 +587,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1024"/>
+  <dimension ref="A1:H1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -865,22 +854,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -917,16 +906,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
@@ -943,7 +932,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -969,7 +958,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -981,10 +970,10 @@
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -995,22 +984,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1021,22 +1010,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -1053,10 +1042,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>21</v>
@@ -1079,16 +1068,16 @@
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -1125,126 +1114,126 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
@@ -1255,16 +1244,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>151</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
@@ -1280,75 +1269,75 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>52</v>
+      <c r="A18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>158</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
@@ -1359,22 +1348,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
@@ -1385,22 +1374,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
@@ -1420,7 +1409,7 @@
         <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>66</v>
@@ -1436,23 +1425,23 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>73</v>
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>14</v>
@@ -1463,22 +1452,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>153</v>
+        <v>72</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>154</v>
+        <v>73</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>14</v>
@@ -1489,74 +1478,74 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>136</v>
+        <v>147</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>76</v>
+        <v>122</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
@@ -1567,48 +1556,48 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="2" t="s">
         <v>77</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>76</v>
@@ -1618,75 +1607,75 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>14</v>
+      <c r="A31" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>98</v>
+      <c r="D33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
@@ -1697,74 +1686,74 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>14</v>
@@ -1775,111 +1764,109 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="E40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>167</v>
-      </c>
       <c r="G40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C41" s="3"/>
-    </row>
+      <c r="H40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2859,9 +2846,8 @@
     <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
little change to ward haven classifier
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6658F-AAF9-422C-90BF-FF24237667C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5547EAC6-618C-4228-8E7B-DFFD2C974887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -325,12 +325,6 @@
     <t>74zWS</t>
   </si>
   <si>
-    <t>Enchanted Knight</t>
-  </si>
-  <si>
-    <t>74sBi</t>
-  </si>
-  <si>
     <t>Artifact Portal</t>
   </si>
   <si>
@@ -542,6 +536,12 @@
   </si>
   <si>
     <t>Illganeau Portal</t>
+  </si>
+  <si>
+    <t>Wilbert, Grand Knight</t>
+  </si>
+  <si>
+    <t>6vX5I</t>
   </si>
 </sst>
 </file>
@@ -809,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -854,22 +854,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -906,16 +906,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
@@ -932,7 +932,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -970,10 +970,10 @@
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -984,22 +984,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1010,22 +1010,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -1042,10 +1042,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>21</v>
@@ -1068,16 +1068,16 @@
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -1114,22 +1114,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="E12" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>28</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>48</v>
@@ -1409,7 +1409,7 @@
         <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>66</v>
@@ -1452,16 +1452,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>72</v>
@@ -1490,10 +1490,10 @@
         <v>71</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>14</v>
@@ -1504,48 +1504,48 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>75</v>
@@ -1608,22 +1608,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>76</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>87</v>
@@ -1672,10 +1672,10 @@
         <v>89</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
@@ -1718,10 +1718,10 @@
         <v>87</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>96</v>
@@ -1750,10 +1750,10 @@
         <v>100</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>14</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>87</v>
@@ -1776,10 +1776,10 @@
         <v>89</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
@@ -1790,22 +1790,22 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>14</v>
@@ -1816,22 +1816,22 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>14</v>
@@ -1842,22 +1842,22 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Bugfix : Duplicate name handling and Meta Updates
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5547EAC6-618C-4228-8E7B-DFFD2C974887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA8EFB9-7FA2-4A4F-A212-1D51A8372699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="180">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -73,33 +73,12 @@
     <t>72h1S</t>
   </si>
   <si>
-    <t>Lucifer, Fallen Angel</t>
-  </si>
-  <si>
-    <t>72Ico</t>
-  </si>
-  <si>
-    <t>Aggro Sword</t>
-  </si>
-  <si>
     <t>Sword</t>
   </si>
   <si>
-    <t>Quickblader</t>
-  </si>
-  <si>
-    <t>5-Hb2</t>
-  </si>
-  <si>
     <t>Evo Sword</t>
   </si>
   <si>
-    <t>Alyaska, War Hawker</t>
-  </si>
-  <si>
-    <t>6_FJ6</t>
-  </si>
-  <si>
     <t>Kagemitsu, Matchless Blade</t>
   </si>
   <si>
@@ -271,12 +250,6 @@
     <t>Control Blood</t>
   </si>
   <si>
-    <t>Illya, Queen of Night</t>
-  </si>
-  <si>
-    <t>6v8gy</t>
-  </si>
-  <si>
     <t>Nerea, Beast Empress</t>
   </si>
   <si>
@@ -310,12 +283,6 @@
     <t>Natura Haven</t>
   </si>
   <si>
-    <t>Agnes, Hollow Feather</t>
-  </si>
-  <si>
-    <t>6rgWC</t>
-  </si>
-  <si>
     <t>Ward Haven</t>
   </si>
   <si>
@@ -355,18 +322,12 @@
     <t>75EcC</t>
   </si>
   <si>
-    <t>fskF2</t>
-  </si>
-  <si>
     <t>6-qS2</t>
   </si>
   <si>
     <t>Chipper Skipper</t>
   </si>
   <si>
-    <t>Control Heal Haven</t>
-  </si>
-  <si>
     <t>Holy Sanctuary</t>
   </si>
   <si>
@@ -424,124 +385,181 @@
     <t>Control Ra Haven</t>
   </si>
   <si>
+    <t>Control OTK Portal</t>
+  </si>
+  <si>
+    <t>Snnneak Attack!</t>
+  </si>
+  <si>
+    <t>6rc6o</t>
+  </si>
+  <si>
+    <t>Karyl Rune</t>
+  </si>
+  <si>
+    <t>Grudge Teller</t>
+  </si>
+  <si>
+    <t>745MY</t>
+  </si>
+  <si>
+    <t>Gremory Shadow</t>
+  </si>
+  <si>
+    <t>Gremory, Death Teller</t>
+  </si>
+  <si>
+    <t>6yaPI</t>
+  </si>
+  <si>
+    <t>Valdain Roost Dragon</t>
+  </si>
+  <si>
+    <t>XII. Wolfraud, Hanged Man</t>
+  </si>
+  <si>
+    <t>6-suI</t>
+  </si>
+  <si>
+    <t>Princess Knight</t>
+  </si>
+  <si>
+    <t>6spli</t>
+  </si>
+  <si>
+    <t>Hanged Man Forest</t>
+  </si>
+  <si>
+    <t>6zcK2</t>
+  </si>
+  <si>
+    <t>Android Artisan</t>
+  </si>
+  <si>
+    <t>Varmint Hunter</t>
+  </si>
+  <si>
+    <t>72c8y</t>
+  </si>
+  <si>
+    <t>Baal Blood</t>
+  </si>
+  <si>
+    <t>Wrath Blood</t>
+  </si>
+  <si>
+    <t>Scrappy Werewolf</t>
+  </si>
+  <si>
+    <t>74Tn2</t>
+  </si>
+  <si>
+    <t>Darhold, Abyssal Contract</t>
+  </si>
+  <si>
+    <t>70myy</t>
+  </si>
+  <si>
+    <t>Bayleon, Sovereign Light</t>
+  </si>
+  <si>
+    <t>Natura Sword</t>
+  </si>
+  <si>
+    <t>6poty</t>
+  </si>
+  <si>
+    <t>6zhxQ</t>
+  </si>
+  <si>
+    <t>Rebel Against Fate</t>
+  </si>
+  <si>
+    <t>Wilbert, Grand Knight</t>
+  </si>
+  <si>
+    <t>6vX5I</t>
+  </si>
+  <si>
+    <t>Rally Portal</t>
+  </si>
+  <si>
+    <t>6rbds</t>
+  </si>
+  <si>
+    <t>Saintly Squeaks</t>
+  </si>
+  <si>
+    <t>Walfrid Sword</t>
+  </si>
+  <si>
+    <t>Walfrid, Sky Captain</t>
+  </si>
+  <si>
+    <t>733S6</t>
+  </si>
+  <si>
+    <t>Amelia, the Silverflash</t>
+  </si>
+  <si>
+    <t>6xRA6</t>
+  </si>
+  <si>
+    <t>Radical Gunslinger</t>
+  </si>
+  <si>
+    <t>730_i</t>
+  </si>
+  <si>
+    <t>Fieran, Havensent Wind God</t>
+  </si>
+  <si>
+    <t>6-UTy</t>
+  </si>
+  <si>
+    <t>Luxblade Arriet</t>
+  </si>
+  <si>
+    <t>6td16</t>
+  </si>
+  <si>
+    <t>Bloodtroth Epitaph</t>
+  </si>
+  <si>
+    <t>74Z8o</t>
+  </si>
+  <si>
+    <t>Sanctuary Haven</t>
+  </si>
+  <si>
+    <t>Aggro-Rally Sword</t>
+  </si>
+  <si>
+    <t>W-A-V Blood</t>
+  </si>
+  <si>
+    <t>Lionel, Woodland Shadow</t>
+  </si>
+  <si>
+    <t>6-qSC</t>
+  </si>
+  <si>
+    <t>Bloodsoaked Archdemon</t>
+  </si>
+  <si>
+    <t>74b66</t>
+  </si>
+  <si>
+    <t>Accelerate Forest</t>
+  </si>
+  <si>
     <t>Aggro Forest</t>
   </si>
   <si>
-    <t>Shamu &amp; Shama, Posh Felines</t>
-  </si>
-  <si>
-    <t>72h1I</t>
-  </si>
-  <si>
-    <t>Stroke of Conviction</t>
-  </si>
-  <si>
-    <t>6xPSQ</t>
-  </si>
-  <si>
-    <t>Control OTK Portal</t>
-  </si>
-  <si>
-    <t>Snnneak Attack!</t>
-  </si>
-  <si>
-    <t>6rc6o</t>
-  </si>
-  <si>
-    <t>Karyl Rune</t>
-  </si>
-  <si>
-    <t>Evo Forest</t>
-  </si>
-  <si>
-    <t>Grudge Teller</t>
-  </si>
-  <si>
-    <t>745MY</t>
-  </si>
-  <si>
-    <t>Gremory Shadow</t>
-  </si>
-  <si>
-    <t>Gremory, Death Teller</t>
-  </si>
-  <si>
-    <t>6yaPI</t>
-  </si>
-  <si>
-    <t>Valdain Roost Dragon</t>
-  </si>
-  <si>
-    <t>XII. Wolfraud, Hanged Man</t>
-  </si>
-  <si>
-    <t>6-suI</t>
-  </si>
-  <si>
-    <t>Princess Knight</t>
-  </si>
-  <si>
-    <t>6spli</t>
-  </si>
-  <si>
-    <t>Hanged Man Forest</t>
-  </si>
-  <si>
-    <t>6zcK2</t>
-  </si>
-  <si>
-    <t>Android Artisan</t>
-  </si>
-  <si>
-    <t>Varmint Hunter</t>
-  </si>
-  <si>
-    <t>72c8y</t>
-  </si>
-  <si>
-    <t>Tempo Forest</t>
-  </si>
-  <si>
-    <t>Baal Blood</t>
-  </si>
-  <si>
-    <t>Wrath Blood</t>
-  </si>
-  <si>
-    <t>Scrappy Werewolf</t>
-  </si>
-  <si>
-    <t>74Tn2</t>
-  </si>
-  <si>
-    <t>Darhold, Abyssal Contract</t>
-  </si>
-  <si>
-    <t>70myy</t>
-  </si>
-  <si>
-    <t>Bayleon, Sovereign Light</t>
-  </si>
-  <si>
-    <t>Natura Sword</t>
-  </si>
-  <si>
-    <t>6poty</t>
-  </si>
-  <si>
-    <t>6zhxQ</t>
-  </si>
-  <si>
-    <t>Rebel Against Fate</t>
-  </si>
-  <si>
-    <t>Illganeau Portal</t>
-  </si>
-  <si>
-    <t>Wilbert, Grand Knight</t>
-  </si>
-  <si>
-    <t>6vX5I</t>
+    <t>Nahtnaught, Cursed Queen</t>
+  </si>
+  <si>
+    <t>733Ry</t>
   </si>
 </sst>
 </file>
@@ -809,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -854,22 +872,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -905,23 +923,23 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
@@ -932,22 +950,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>172</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>173</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -958,22 +976,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>139</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -983,23 +1001,23 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>158</v>
+      <c r="C7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1010,74 +1028,74 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>161</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>162</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -1088,22 +1106,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>147</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>26</v>
+        <v>148</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>27</v>
+        <v>148</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
@@ -1114,80 +1132,80 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>167</v>
+        <v>112</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>166</v>
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>166</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>168</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1195,7 +1213,7 @@
         <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>37</v>
@@ -1204,36 +1222,36 @@
         <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
@@ -1244,99 +1262,99 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>40</v>
+      <c r="D18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -1348,22 +1366,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
@@ -1374,22 +1392,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
@@ -1400,48 +1418,48 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>14</v>
@@ -1452,22 +1470,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>146</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>147</v>
+        <v>63</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>148</v>
+        <v>64</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>14</v>
@@ -1478,74 +1496,74 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>14</v>
+        <v>108</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>127</v>
+        <v>108</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
@@ -1556,126 +1574,126 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>14</v>
+      <c r="G29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>161</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>163</v>
+        <v>77</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>82</v>
+        <v>171</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>85</v>
+        <v>167</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>77</v>
+        <v>168</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>169</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
@@ -1686,22 +1704,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
@@ -1712,22 +1730,22 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
@@ -1738,22 +1756,22 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>14</v>
@@ -1764,22 +1782,22 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
@@ -1790,22 +1808,22 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>14</v>
@@ -1816,48 +1834,48 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>14</v>
+        <v>99</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Bugfix : Fixed duplicate name problem for JCG Qualified Top 16
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA8EFB9-7FA2-4A4F-A212-1D51A8372699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA38042-8AFB-486C-B658-AC905528DC60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="196">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -217,12 +217,6 @@
     <t>748Xg</t>
   </si>
   <si>
-    <t>Invincible Monster Trio</t>
-  </si>
-  <si>
-    <t>74ChS</t>
-  </si>
-  <si>
     <t>Highlander Blood</t>
   </si>
   <si>
@@ -310,12 +304,6 @@
     <t>6s65g</t>
   </si>
   <si>
-    <t>Illganeau, Horror Astray</t>
-  </si>
-  <si>
-    <t>75Lwo</t>
-  </si>
-  <si>
     <t>Stringmaster</t>
   </si>
   <si>
@@ -560,6 +548,66 @@
   </si>
   <si>
     <t>733Ry</t>
+  </si>
+  <si>
+    <t>Sarcophagus Wraith</t>
+  </si>
+  <si>
+    <t>6yXzC</t>
+  </si>
+  <si>
+    <t>Heal Blood</t>
+  </si>
+  <si>
+    <t>Craps Devil</t>
+  </si>
+  <si>
+    <t>74WDI</t>
+  </si>
+  <si>
+    <t>Ruinweb Spider</t>
+  </si>
+  <si>
+    <t>6yyq6</t>
+  </si>
+  <si>
+    <t>Jerva Dragon</t>
+  </si>
+  <si>
+    <t>Jerva, Wyrm Transcendent</t>
+  </si>
+  <si>
+    <t>6yB_6</t>
+  </si>
+  <si>
+    <t>Encounter from the Deep</t>
+  </si>
+  <si>
+    <t>73oZQ</t>
+  </si>
+  <si>
+    <t>Vehicle Dragon</t>
+  </si>
+  <si>
+    <t>Quixotic Adventurer</t>
+  </si>
+  <si>
+    <t>72BIC</t>
+  </si>
+  <si>
+    <t>Reggie, Peerless Artisan</t>
+  </si>
+  <si>
+    <t>73qGy</t>
+  </si>
+  <si>
+    <t>West Wind Haven</t>
+  </si>
+  <si>
+    <t>Goddess of the West Wind</t>
+  </si>
+  <si>
+    <t>6vX5c</t>
   </si>
 </sst>
 </file>
@@ -614,7 +662,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -825,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1023"/>
+  <dimension ref="A1:H1027"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -872,22 +928,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -924,7 +980,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -950,22 +1006,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -976,22 +1032,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -1002,22 +1058,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1028,54 +1084,54 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1086,10 +1142,10 @@
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>
@@ -1106,22 +1162,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
@@ -1132,7 +1188,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
@@ -1262,7 +1318,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
@@ -1314,7 +1370,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>41</v>
@@ -1401,7 +1457,7 @@
         <v>57</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>59</v>
@@ -1443,23 +1499,23 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>66</v>
+      <c r="A24" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>14</v>
@@ -1469,23 +1525,23 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>126</v>
+      <c r="A25" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>14</v>
@@ -1496,48 +1552,48 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>114</v>
+        <v>177</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>14</v>
@@ -1548,346 +1604,446 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>14</v>
+        <v>104</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>14</v>
+      <c r="A33" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>82</v>
+        <v>170</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>14</v>
+        <v>75</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="D39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="E40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B39" s="1" t="s">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="F44" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2864,6 +3020,10 @@
     <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1026" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1027" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feature : more stats for conversion rate
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/StormOverRivayleMeta.xlsx
+++ b/Excel_and_CSV/StormOverRivayleMeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74809FC0-6FF5-47AF-B414-C6D16B2EC9C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F0A230-8A96-489C-810F-19239EF3F549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,12 +553,6 @@
     <t>74WDI</t>
   </si>
   <si>
-    <t>Ruinweb Spider</t>
-  </si>
-  <si>
-    <t>6yyq6</t>
-  </si>
-  <si>
     <t>Jerva Dragon</t>
   </si>
   <si>
@@ -608,6 +602,12 @@
   </si>
   <si>
     <t>72Zis</t>
+  </si>
+  <si>
+    <t>Fulminating Berserker</t>
+  </si>
+  <si>
+    <t>74TnC</t>
   </si>
 </sst>
 </file>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1030,16 +1030,16 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -1166,10 +1166,10 @@
         <v>158</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
@@ -1518,22 +1518,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>14</v>
@@ -1544,22 +1544,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>14</v>
@@ -1764,10 +1764,10 @@
         <v>176</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>67</v>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>76</v>
@@ -1972,10 +1972,10 @@
         <v>83</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>14</v>

</xml_diff>